<commit_message>
Add functional to export both summary and description in excel.
</commit_message>
<xml_diff>
--- a/Estimation.WebApi/Forms/SummaryOfEstimation_SubmitForm.xlsx
+++ b/Estimation.WebApi/Forms/SummaryOfEstimation_SubmitForm.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattanapol.K\source\repos\EstimationServer\Estimation.WebApi\Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mattanapol.K\Source\Repos\EstimationServer\Estimation.WebApi\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{85EBF415-FF9E-4791-AAE3-C4D0A403FFE1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -89,7 +90,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -374,83 +375,83 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -765,11 +766,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -783,15 +784,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -816,113 +817,113 @@
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:8" s="4" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10"/>
-      <c r="B5" s="11" t="s">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="13"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="16">
+      <c r="C6" s="15">
         <v>1</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17" t="s">
+      <c r="E6" s="16"/>
+      <c r="F6" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="13"/>
+      <c r="B7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="16">
+      <c r="C7" s="15">
         <v>1</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="17"/>
-      <c r="G7" s="18" t="s">
+      <c r="F7" s="16"/>
+      <c r="G7" s="17" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="19" t="s">
+      <c r="A8" s="13"/>
+      <c r="B8" s="16"/>
+      <c r="C8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="20" t="s">
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="G8" s="31"/>
+      <c r="G8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="29"/>
-      <c r="F9" s="29"/>
-      <c r="G9" s="30"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="27"/>
     </row>
     <row r="10" spans="1:8" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="21"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="23" t="s">
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="31" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="23"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="24" t="s">
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="25"/>
+      <c r="G10" s="22"/>
     </row>
     <row r="11" spans="1:8" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>

</xml_diff>